<commit_message>
I added a loading form. I also updated the style and used a custom text box. The transparent style failed
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,6 +528,539 @@
         <v>40</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42601.700833333336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>3287</v>
+      </c>
+      <c r="D4">
+        <v>6859</v>
+      </c>
+      <c r="E4">
+        <v>844</v>
+      </c>
+      <c r="F4">
+        <v>187</v>
+      </c>
+      <c r="G4">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>80</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42601.73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>3724</v>
+      </c>
+      <c r="D5">
+        <v>6866</v>
+      </c>
+      <c r="E5">
+        <v>844</v>
+      </c>
+      <c r="F5">
+        <v>188</v>
+      </c>
+      <c r="G5">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>80</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42601.731319444443</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>3570</v>
+      </c>
+      <c r="D6">
+        <v>6640</v>
+      </c>
+      <c r="E6">
+        <v>817</v>
+      </c>
+      <c r="F6">
+        <v>182</v>
+      </c>
+      <c r="G6">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42601.740636574075</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>3592</v>
+      </c>
+      <c r="D7">
+        <v>6641</v>
+      </c>
+      <c r="E7">
+        <v>817</v>
+      </c>
+      <c r="F7">
+        <v>181</v>
+      </c>
+      <c r="G7">
+        <v>42</v>
+      </c>
+      <c r="H7">
+        <v>79</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42601.743159722224</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>5192</v>
+      </c>
+      <c r="D8">
+        <v>6640</v>
+      </c>
+      <c r="E8">
+        <v>817</v>
+      </c>
+      <c r="F8">
+        <v>182</v>
+      </c>
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>80</v>
+      </c>
+      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42601.745439814818</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>3676</v>
+      </c>
+      <c r="D9">
+        <v>6630</v>
+      </c>
+      <c r="E9">
+        <v>815</v>
+      </c>
+      <c r="F9">
+        <v>182</v>
+      </c>
+      <c r="G9">
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <v>80</v>
+      </c>
+      <c r="I9">
+        <v>18</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42601.746759259258</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>3682</v>
+      </c>
+      <c r="D10">
+        <v>6640</v>
+      </c>
+      <c r="E10">
+        <v>817</v>
+      </c>
+      <c r="F10">
+        <v>182</v>
+      </c>
+      <c r="G10">
+        <v>42</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42601.754016203704</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>3666</v>
+      </c>
+      <c r="D11">
+        <v>6640</v>
+      </c>
+      <c r="E11">
+        <v>816</v>
+      </c>
+      <c r="F11">
+        <v>182</v>
+      </c>
+      <c r="G11">
+        <v>42</v>
+      </c>
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42601.756493055553</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>3620</v>
+      </c>
+      <c r="D12">
+        <v>6633</v>
+      </c>
+      <c r="E12">
+        <v>816</v>
+      </c>
+      <c r="F12">
+        <v>182</v>
+      </c>
+      <c r="G12">
+        <v>42</v>
+      </c>
+      <c r="H12">
+        <v>80</v>
+      </c>
+      <c r="I12">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42601.757418981484</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>3573</v>
+      </c>
+      <c r="D13">
+        <v>6632</v>
+      </c>
+      <c r="E13">
+        <v>816</v>
+      </c>
+      <c r="F13">
+        <v>182</v>
+      </c>
+      <c r="G13">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <v>80</v>
+      </c>
+      <c r="I13">
+        <v>18</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42601.759988425925</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>4295</v>
+      </c>
+      <c r="D14">
+        <v>6640</v>
+      </c>
+      <c r="E14">
+        <v>817</v>
+      </c>
+      <c r="F14">
+        <v>182</v>
+      </c>
+      <c r="G14">
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <v>80</v>
+      </c>
+      <c r="I14">
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42601.762928240743</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>3646</v>
+      </c>
+      <c r="D15">
+        <v>6640</v>
+      </c>
+      <c r="E15">
+        <v>817</v>
+      </c>
+      <c r="F15">
+        <v>181</v>
+      </c>
+      <c r="G15">
+        <v>42</v>
+      </c>
+      <c r="H15">
+        <v>79</v>
+      </c>
+      <c r="I15">
+        <v>18</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42601.775763888887</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>4035</v>
+      </c>
+      <c r="D16">
+        <v>7043</v>
+      </c>
+      <c r="E16">
+        <v>878</v>
+      </c>
+      <c r="F16">
+        <v>175</v>
+      </c>
+      <c r="G16">
+        <v>47</v>
+      </c>
+      <c r="H16">
+        <v>78</v>
+      </c>
+      <c r="I16">
+        <v>21</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the look of the loading window
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1061,6 +1061,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42602.010092592594</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>5860</v>
+      </c>
+      <c r="D17">
+        <v>6487</v>
+      </c>
+      <c r="E17">
+        <v>815</v>
+      </c>
+      <c r="F17">
+        <v>130</v>
+      </c>
+      <c r="G17">
+        <v>59</v>
+      </c>
+      <c r="H17">
+        <v>67</v>
+      </c>
+      <c r="I17">
+        <v>30</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42602.481874999998</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>5803</v>
+      </c>
+      <c r="D18">
+        <v>9336</v>
+      </c>
+      <c r="E18">
+        <v>1178</v>
+      </c>
+      <c r="F18">
+        <v>193</v>
+      </c>
+      <c r="G18">
+        <v>101</v>
+      </c>
+      <c r="H18">
+        <v>65</v>
+      </c>
+      <c r="I18">
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the total score function
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
@@ -29,40 +29,40 @@
     <t>Date</t>
   </si>
   <si>
+    <t>posWordPercentage</t>
+  </si>
+  <si>
+    <t>negWordPercentage</t>
+  </si>
+  <si>
+    <t>posPhrasePercentage</t>
+  </si>
+  <si>
+    <t>negPhrasePercentage</t>
+  </si>
+  <si>
+    <t>ElapsedMs</t>
+  </si>
+  <si>
+    <t>wordCount</t>
+  </si>
+  <si>
+    <t>sentenceCount</t>
+  </si>
+  <si>
+    <t>posWordCount</t>
+  </si>
+  <si>
+    <t>negWordCount</t>
+  </si>
+  <si>
+    <t>positivePhraseCount</t>
+  </si>
+  <si>
+    <t>negativePhraseCount</t>
+  </si>
+  <si>
     <t>Method</t>
-  </si>
-  <si>
-    <t>ElapsedMs</t>
-  </si>
-  <si>
-    <t>wordCount</t>
-  </si>
-  <si>
-    <t>sentenceCount</t>
-  </si>
-  <si>
-    <t>posWordCount</t>
-  </si>
-  <si>
-    <t>negWordCount</t>
-  </si>
-  <si>
-    <t>posWordPercentage</t>
-  </si>
-  <si>
-    <t>negWordPercentage</t>
-  </si>
-  <si>
-    <t>positivePhraseCount</t>
-  </si>
-  <si>
-    <t>negativePhraseCount</t>
-  </si>
-  <si>
-    <t>posPhrasePercentage</t>
-  </si>
-  <si>
-    <t>negPhrasePercentage</t>
   </si>
   <si>
     <t>Bag</t>
@@ -391,18 +391,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -448,43 +448,43 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42603.707488425927</v>
-      </c>
-      <c r="B2" t="s">
+        <v>42605.455081018517</v>
+      </c>
+      <c r="B2">
+        <v>66</v>
+      </c>
+      <c r="C2">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>91</v>
+      </c>
+      <c r="F2">
+        <v>4443</v>
+      </c>
+      <c r="G2">
+        <v>6623</v>
+      </c>
+      <c r="H2">
+        <v>762</v>
+      </c>
+      <c r="I2">
+        <v>152</v>
+      </c>
+      <c r="J2">
+        <v>71</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added excel functionality. Sped up the whole application
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/CLNE/CLNEBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -496,6 +496,358 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42606.52685185185</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>75</v>
+      </c>
+      <c r="G3">
+        <v>1882</v>
+      </c>
+      <c r="H3">
+        <v>3360</v>
+      </c>
+      <c r="I3">
+        <v>427</v>
+      </c>
+      <c r="J3">
+        <v>73</v>
+      </c>
+      <c r="K3">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42606.542592592596</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>75</v>
+      </c>
+      <c r="G4">
+        <v>1568</v>
+      </c>
+      <c r="H4">
+        <v>3367</v>
+      </c>
+      <c r="I4">
+        <v>427</v>
+      </c>
+      <c r="J4">
+        <v>73</v>
+      </c>
+      <c r="K4">
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42606.551504629628</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>75</v>
+      </c>
+      <c r="G5">
+        <v>1695</v>
+      </c>
+      <c r="H5">
+        <v>3367</v>
+      </c>
+      <c r="I5">
+        <v>427</v>
+      </c>
+      <c r="J5">
+        <v>73</v>
+      </c>
+      <c r="K5">
+        <v>24</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42606.554189814815</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>75</v>
+      </c>
+      <c r="G6">
+        <v>1592</v>
+      </c>
+      <c r="H6">
+        <v>3367</v>
+      </c>
+      <c r="I6">
+        <v>427</v>
+      </c>
+      <c r="J6">
+        <v>73</v>
+      </c>
+      <c r="K6">
+        <v>24</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42606.555902777778</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>75</v>
+      </c>
+      <c r="G7">
+        <v>1629</v>
+      </c>
+      <c r="H7">
+        <v>3369</v>
+      </c>
+      <c r="I7">
+        <v>427</v>
+      </c>
+      <c r="J7">
+        <v>73</v>
+      </c>
+      <c r="K7">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42606.55945601852</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>1632</v>
+      </c>
+      <c r="H8">
+        <v>3367</v>
+      </c>
+      <c r="I8">
+        <v>427</v>
+      </c>
+      <c r="J8">
+        <v>73</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42606.566932870373</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>75</v>
+      </c>
+      <c r="G9">
+        <v>1522</v>
+      </c>
+      <c r="H9">
+        <v>3367</v>
+      </c>
+      <c r="I9">
+        <v>427</v>
+      </c>
+      <c r="J9">
+        <v>73</v>
+      </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42606.571203703701</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>1560</v>
+      </c>
+      <c r="H10">
+        <v>3367</v>
+      </c>
+      <c r="I10">
+        <v>427</v>
+      </c>
+      <c r="J10">
+        <v>73</v>
+      </c>
+      <c r="K10">
+        <v>24</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>